<commit_message>
Update week-10 Stand-up meeting templet.
</commit_message>
<xml_diff>
--- a/Project_Files/GDP-02-Sprint10/Stand-up Meeting Sec03Team05 Sprint10.xlsx
+++ b/Project_Files/GDP-02-Sprint10/Stand-up Meeting Sec03Team05 Sprint10.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S547076\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S547049\Documents\GitHub\FreebiesforNewbies\Project_Files\GDP-02-Sprint10\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0875AAB8-683F-4301-99D9-FC94DB4170EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D3620AE-1E14-4DEA-BA31-CE95CCBF1604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="380" windowWidth="19180" windowHeight="9780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
   <si>
     <t>Daily Stand-up Meeting Report</t>
   </si>
@@ -142,12 +142,30 @@
 2.What will I do today?
 3.What obstacles are impeding my progress?</t>
   </si>
+  <si>
+    <t>I have did few changes on code to fix errors.</t>
+  </si>
+  <si>
+    <t>I have written backend code for User profile page.</t>
+  </si>
+  <si>
+    <t>I have fixed erros.</t>
+  </si>
+  <si>
+    <t>I will write backend code on user profile page.</t>
+  </si>
+  <si>
+    <t>I will fix errors.</t>
+  </si>
+  <si>
+    <t>I will prepare blueprint for documentation.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -214,6 +232,12 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF252525"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -242,18 +266,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
+        <fgColor theme="0"/>
+        <bgColor theme="0"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor theme="0"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -555,11 +579,71 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
@@ -592,10 +676,9 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -628,6 +711,18 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -845,8 +940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -860,14 +955,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="29"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="28"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -890,12 +985,12 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A2" s="25"/>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="26"/>
+      <c r="A2" s="24"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="25"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -918,14 +1013,14 @@
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="33"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="32"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -948,14 +1043,14 @@
       <c r="Z3" s="1"/>
     </row>
     <row r="4" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="32"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="33"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="32"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -978,14 +1073,14 @@
       <c r="Z4" s="1"/>
     </row>
     <row r="5" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="32"/>
-      <c r="C5" s="32"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="33"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="32"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -1070,7 +1165,7 @@
       <c r="Z7" s="1"/>
     </row>
     <row r="8" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A8" s="35" t="s">
+      <c r="A8" s="34" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="4"/>
@@ -1102,7 +1197,7 @@
       <c r="Z8" s="1"/>
     </row>
     <row r="9" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A9" s="36"/>
+      <c r="A9" s="35"/>
       <c r="B9" s="8"/>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
@@ -1130,7 +1225,7 @@
       <c r="Z9" s="1"/>
     </row>
     <row r="10" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A10" s="37"/>
+      <c r="A10" s="36"/>
       <c r="B10" s="8"/>
       <c r="C10" s="10"/>
       <c r="D10" s="11"/>
@@ -1158,7 +1253,7 @@
       <c r="Z10" s="1"/>
     </row>
     <row r="11" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="17" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="12"/>
@@ -1188,7 +1283,7 @@
       <c r="Z11" s="1"/>
     </row>
     <row r="12" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A12" s="19"/>
+      <c r="A12" s="18"/>
       <c r="B12" s="12"/>
       <c r="C12" s="12"/>
       <c r="D12" s="12"/>
@@ -1215,8 +1310,8 @@
       <c r="Y12" s="1"/>
       <c r="Z12" s="1"/>
     </row>
-    <row r="13" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A13" s="20"/>
+    <row r="13" spans="1:26" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A13" s="19"/>
       <c r="B13" s="12"/>
       <c r="C13" s="12"/>
       <c r="D13" s="12"/>
@@ -1243,12 +1338,19 @@
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
     </row>
-    <row r="14" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A14" s="18" t="s">
+    <row r="14" spans="1:26" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A14" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
+      <c r="B14" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="38" t="s">
+        <v>24</v>
+      </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
@@ -1272,11 +1374,17 @@
       <c r="Y14" s="1"/>
       <c r="Z14" s="1"/>
     </row>
-    <row r="15" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A15" s="19"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="13"/>
+    <row r="15" spans="1:26" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A15" s="18"/>
+      <c r="B15" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="40" t="s">
+        <v>27</v>
+      </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
@@ -1300,11 +1408,17 @@
       <c r="Y15" s="1"/>
       <c r="Z15" s="1"/>
     </row>
-    <row r="16" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A16" s="20"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
+    <row r="16" spans="1:26" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A16" s="19"/>
+      <c r="B16" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="40" t="s">
+        <v>12</v>
+      </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
@@ -1329,7 +1443,7 @@
       <c r="Z16" s="1"/>
     </row>
     <row r="17" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A17" s="18" t="s">
+      <c r="A17" s="17" t="s">
         <v>11</v>
       </c>
       <c r="B17" s="12"/>
@@ -1359,10 +1473,10 @@
       <c r="Z17" s="1"/>
     </row>
     <row r="18" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A18" s="19"/>
+      <c r="A18" s="18"/>
       <c r="B18" s="12"/>
       <c r="C18" s="12"/>
-      <c r="D18" s="15"/>
+      <c r="D18" s="14"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
@@ -1387,7 +1501,7 @@
       <c r="Z18" s="1"/>
     </row>
     <row r="19" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A19" s="20"/>
+      <c r="A19" s="19"/>
       <c r="B19" s="12"/>
       <c r="C19" s="12"/>
       <c r="D19" s="12"/>
@@ -1415,7 +1529,7 @@
       <c r="Z19" s="1"/>
     </row>
     <row r="20" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A20" s="18" t="s">
+      <c r="A20" s="17" t="s">
         <v>13</v>
       </c>
       <c r="B20" s="13" t="s">
@@ -1451,7 +1565,7 @@
       <c r="Z20" s="1"/>
     </row>
     <row r="21" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A21" s="19"/>
+      <c r="A21" s="18"/>
       <c r="B21" s="13" t="s">
         <v>17</v>
       </c>
@@ -1485,7 +1599,7 @@
       <c r="Z21" s="1"/>
     </row>
     <row r="22" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A22" s="20"/>
+      <c r="A22" s="19"/>
       <c r="B22" s="13" t="s">
         <v>12</v>
       </c>
@@ -1575,10 +1689,10 @@
       <c r="Z24" s="1"/>
     </row>
     <row r="25" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A25" s="16" t="s">
+      <c r="A25" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B25" s="17"/>
+      <c r="B25" s="16"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
@@ -1605,10 +1719,10 @@
       <c r="Z25" s="1"/>
     </row>
     <row r="26" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A26" s="21" t="s">
+      <c r="A26" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="B26" s="22"/>
+      <c r="B26" s="21"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
@@ -1635,8 +1749,8 @@
       <c r="Z26" s="1"/>
     </row>
     <row r="27" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A27" s="23"/>
-      <c r="B27" s="24"/>
+      <c r="A27" s="22"/>
+      <c r="B27" s="23"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
@@ -1663,8 +1777,8 @@
       <c r="Z27" s="1"/>
     </row>
     <row r="28" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A28" s="25"/>
-      <c r="B28" s="26"/>
+      <c r="A28" s="24"/>
+      <c r="B28" s="25"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
@@ -28920,6 +29034,6 @@
     <mergeCell ref="A14:A16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>